<commit_message>
Changes made in the process of finalizing diversityMetrics.R
</commit_message>
<xml_diff>
--- a/data-raw/FBSData/FBStoIMPACTlookupV3.xlsx
+++ b/data-raw/FBSData/FBStoIMPACTlookupV3.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutrientModeling/data-raw/FBSData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/FBSData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-24240" yWindow="-5220" windowWidth="22540" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="-24240" yWindow="-6740" windowWidth="22540" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="269">
   <si>
     <t>Alcohol, Non-Food</t>
   </si>
@@ -828,6 +831,9 @@
   </si>
   <si>
     <t>c_aqpl</t>
+  </si>
+  <si>
+    <t>updated March 1, 2017</t>
   </si>
 </sst>
 </file>
@@ -1357,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,7 +1691,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="42" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2657</v>
       </c>
@@ -1696,16 +1702,19 @@
         <v>19</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2655</v>
       </c>
@@ -1725,7 +1734,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2615</v>
       </c>
@@ -1742,7 +1751,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="42" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2513</v>
       </c>
@@ -1759,7 +1768,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2546</v>
       </c>
@@ -1776,7 +1785,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="84" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="84" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2731</v>
       </c>
@@ -1793,7 +1802,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="70" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="70" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2735</v>
       </c>
@@ -1810,7 +1819,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="98" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="98" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2736</v>
       </c>
@@ -1827,7 +1836,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="56" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="56" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2740</v>
       </c>
@@ -1844,7 +1853,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="98" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="98" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2737</v>
       </c>
@@ -1861,7 +1870,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2630</v>
       </c>
@@ -1878,7 +1887,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2532</v>
       </c>
@@ -1895,7 +1904,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2633</v>
       </c>
@@ -1912,7 +1921,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="42" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2744</v>
       </c>
@@ -1929,7 +1938,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2572</v>
       </c>
@@ -1946,7 +1955,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="42" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2556</v>
       </c>

</xml_diff>